<commit_message>
Updated parts list and some values, added to digikey list
Updated parts list and some values, added to digikey list
</commit_message>
<xml_diff>
--- a/Hardware/Bill of Materials/Voltmeter BoM.xlsx
+++ b/Hardware/Bill of Materials/Voltmeter BoM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Daniel\Documents\GitHub\Voltmeter\Hardware\Bill of Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3353FC-CCB0-44D7-9613-4F61112B45C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C099E4-A59F-4BB5-97A3-00DD3BA211DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4560" yWindow="960" windowWidth="24240" windowHeight="12645" xr2:uid="{52156BA4-E22B-48AF-8FCC-A50A3973E615}"/>
+    <workbookView xWindow="4560" yWindow="2610" windowWidth="24240" windowHeight="12645" xr2:uid="{52156BA4-E22B-48AF-8FCC-A50A3973E615}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="84">
   <si>
     <t>Voltmeter BoM</t>
   </si>
@@ -56,18 +56,12 @@
     <t>10V</t>
   </si>
   <si>
-    <t>NPN</t>
-  </si>
-  <si>
     <t>60V VceMin</t>
   </si>
   <si>
     <t>PMOS ADC protect</t>
   </si>
   <si>
-    <t>Low RdsOn, Vds at least 60V</t>
-  </si>
-  <si>
     <t>Comparator</t>
   </si>
   <si>
@@ -77,9 +71,6 @@
     <t>ADC</t>
   </si>
   <si>
-    <t>2 channels, SPI</t>
-  </si>
-  <si>
     <t>Comparator in zener</t>
   </si>
   <si>
@@ -89,9 +80,6 @@
     <t>Chosen part</t>
   </si>
   <si>
-    <t>36V</t>
-  </si>
-  <si>
     <t>AC:</t>
   </si>
   <si>
@@ -116,9 +104,6 @@
     <t>https://www.digikey.co.uk/en/products/detail/murata-electronics/RDER72J474MUE1H03A/4771421</t>
   </si>
   <si>
-    <t>47nF, over 500V</t>
-  </si>
-  <si>
     <t>Common:</t>
   </si>
   <si>
@@ -143,36 +128,24 @@
     <t>12 bit, SPI</t>
   </si>
   <si>
-    <t>SRS-1205-2</t>
-  </si>
-  <si>
     <t>MCP3204-CI/P</t>
   </si>
   <si>
     <t>Micro regulator 12-&gt;5v</t>
   </si>
   <si>
-    <t>DC power isolator 12-&gt;5v</t>
-  </si>
-  <si>
     <t>https://www.digikey.co.uk/en/products/detail/stmicroelectronics/L7805CV/585964</t>
   </si>
   <si>
     <t>L7805CV</t>
   </si>
   <si>
-    <t>SPI comms isolator</t>
-  </si>
-  <si>
     <t>https://www.digikey.co.uk/en/products/detail/liteon/LTV-849/3199522</t>
   </si>
   <si>
     <t>LTV-849</t>
   </si>
   <si>
-    <t>https://www.digikey.co.uk/en/products/detail/diwell-electronics/SRS-1205-2/16572067</t>
-  </si>
-  <si>
     <t>Power barrel 12v or equivalent</t>
   </si>
   <si>
@@ -180,13 +153,148 @@
   </si>
   <si>
     <t>4 channel opto x2</t>
+  </si>
+  <si>
+    <t>On list?</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>Comms isolator</t>
+  </si>
+  <si>
+    <t>RFM-0505S</t>
+  </si>
+  <si>
+    <t>DC power isolator 5V-&gt;5v</t>
+  </si>
+  <si>
+    <t>https://www.digikey.co.uk/en/products/detail/recom-power/RFM-0505S/8550767</t>
+  </si>
+  <si>
+    <t>ADC channel NMOS</t>
+  </si>
+  <si>
+    <t>ADC channel NPN</t>
+  </si>
+  <si>
+    <t>470nF, over 500V</t>
+  </si>
+  <si>
+    <t>RDER72J474MUE1H03A</t>
+  </si>
+  <si>
+    <t>ZPD5.1</t>
+  </si>
+  <si>
+    <t>43V</t>
+  </si>
+  <si>
+    <t>https://www.digikey.co.uk/en/products/detail/diotec-semiconductor/ZPD43/22192402</t>
+  </si>
+  <si>
+    <t>ZPD43</t>
+  </si>
+  <si>
+    <t>2N7000</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Already have these</t>
+  </si>
+  <si>
+    <t>BC546B</t>
+  </si>
+  <si>
+    <t>https://diotec.com/request/datasheet/bc546.pdf</t>
+  </si>
+  <si>
+    <t>DMP45H4D9HJ3</t>
+  </si>
+  <si>
+    <t>Low RdsOn, Vds at least 400V</t>
+  </si>
+  <si>
+    <t>https://www.digikey.co.uk/en/products/detail/diodes-incorporated/DMP45H4D9HJ3/7666871</t>
+  </si>
+  <si>
+    <t>2Meg Resistor</t>
+  </si>
+  <si>
+    <t>RNF14FTD2M00</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/catalog/sei-rnf_rnmf.pdf</t>
+  </si>
+  <si>
+    <t>1Meg Resistor</t>
+  </si>
+  <si>
+    <t>Already have</t>
+  </si>
+  <si>
+    <t>25k res</t>
+  </si>
+  <si>
+    <t>MFR-25FBF52-5K36</t>
+  </si>
+  <si>
+    <t>287k</t>
+  </si>
+  <si>
+    <t>MFR-25FBF52-287K</t>
+  </si>
+  <si>
+    <t>MF1/4DCT52R1404F</t>
+  </si>
+  <si>
+    <t>1.4Meg</t>
+  </si>
+  <si>
+    <t>200k</t>
+  </si>
+  <si>
+    <t>6.2k</t>
+  </si>
+  <si>
+    <t>MFR-25FRF52-6K2</t>
+  </si>
+  <si>
+    <t>RNV14FAL7M50</t>
+  </si>
+  <si>
+    <t>7.5Meg</t>
+  </si>
+  <si>
+    <t>95.3k</t>
+  </si>
+  <si>
+    <t>MFR-25FBF52-95K3</t>
+  </si>
+  <si>
+    <t>4.7Meg</t>
+  </si>
+  <si>
+    <t>MFR-25FTE52-4M7</t>
+  </si>
+  <si>
+    <t>62k</t>
+  </si>
+  <si>
+    <t>RNMF14FTC62K0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,9 +332,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -562,33 +673,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47E77683-9D70-4467-A4C1-848CD3003F51}">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="1" max="1" width="27.875" customWidth="1"/>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -596,187 +713,435 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" t="s">
+        <v>40</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" t="s">
+        <v>40</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26" t="s">
+        <v>40</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E35" t="s">
+        <v>40</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E36" t="s">
+        <v>40</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" t="s">
+        <v>43</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E37" t="s">
+        <v>40</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" t="s">
-        <v>28</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" t="s">
-        <v>30</v>
-      </c>
-      <c r="D29" s="1" t="s">
+      <c r="C38" t="s">
+        <v>33</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="E38" t="s">
+        <v>40</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" t="s">
+        <v>35</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C30" t="s">
+      <c r="E39" t="s">
+        <v>40</v>
+      </c>
+      <c r="F39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
         <v>36</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>38</v>
-      </c>
-      <c r="C31" t="s">
-        <v>35</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>37</v>
-      </c>
-      <c r="C32" t="s">
-        <v>40</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>41</v>
-      </c>
-      <c r="B33" t="s">
-        <v>47</v>
-      </c>
-      <c r="C33" t="s">
-        <v>43</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D17" r:id="rId1" xr:uid="{53464FBA-EA44-43D6-B9C2-5F375BCE3C5D}"/>
-    <hyperlink ref="D19" r:id="rId2" xr:uid="{AAD82B4C-23E5-486D-8542-0FA27ECECCA7}"/>
-    <hyperlink ref="D18" r:id="rId3" xr:uid="{FBEB51FF-0A39-415C-B202-0AC583177E6F}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{55C85E82-42AD-4A33-B5FF-6B82465F1347}"/>
-    <hyperlink ref="D29" r:id="rId5" xr:uid="{44A2C188-E783-4FA4-B59E-C253D78B761E}"/>
-    <hyperlink ref="D30" r:id="rId6" xr:uid="{C8FCEF85-F6EE-4BCF-A3B7-F0AB55857504}"/>
-    <hyperlink ref="D32" r:id="rId7" xr:uid="{6C742ABE-D945-43E6-A891-8A5D95B26334}"/>
-    <hyperlink ref="D33" r:id="rId8" xr:uid="{80D5FD26-BAA5-4E5C-AB91-B3E54B0AC33F}"/>
-    <hyperlink ref="D31" r:id="rId9" xr:uid="{6C48BD37-4CD8-42B3-97C5-E252B8D1C70A}"/>
-    <hyperlink ref="D28" r:id="rId10" xr:uid="{B7BF6A1C-9D36-4F9A-8673-EF88BFD4ABC5}"/>
+    <hyperlink ref="D23" r:id="rId1" xr:uid="{53464FBA-EA44-43D6-B9C2-5F375BCE3C5D}"/>
+    <hyperlink ref="D25" r:id="rId2" xr:uid="{AAD82B4C-23E5-486D-8542-0FA27ECECCA7}"/>
+    <hyperlink ref="D24" r:id="rId3" xr:uid="{FBEB51FF-0A39-415C-B202-0AC583177E6F}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{55C85E82-42AD-4A33-B5FF-6B82465F1347}"/>
+    <hyperlink ref="D35" r:id="rId5" xr:uid="{44A2C188-E783-4FA4-B59E-C253D78B761E}"/>
+    <hyperlink ref="D36" r:id="rId6" xr:uid="{C8FCEF85-F6EE-4BCF-A3B7-F0AB55857504}"/>
+    <hyperlink ref="D38" r:id="rId7" xr:uid="{6C742ABE-D945-43E6-A891-8A5D95B26334}"/>
+    <hyperlink ref="D39" r:id="rId8" xr:uid="{80D5FD26-BAA5-4E5C-AB91-B3E54B0AC33F}"/>
+    <hyperlink ref="D34" r:id="rId9" xr:uid="{B7BF6A1C-9D36-4F9A-8673-EF88BFD4ABC5}"/>
+    <hyperlink ref="D37" r:id="rId10" xr:uid="{F70B17A7-FC85-45BE-8D2C-1662D80EADD5}"/>
+    <hyperlink ref="D7" r:id="rId11" xr:uid="{34BA19BE-FBDD-4C2C-9CC2-BA4A91211E08}"/>
+    <hyperlink ref="D9" r:id="rId12" xr:uid="{AFBF0F2D-1B2E-4CF6-98A1-52EA3AC47177}"/>
+    <hyperlink ref="D6" r:id="rId13" xr:uid="{0B201D1B-7732-4E2F-A18A-0649593BCC07}"/>
+    <hyperlink ref="D10" r:id="rId14" xr:uid="{2CEDAC28-64E4-46B2-AB25-FA287D3C44B9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>